<commit_message>
inclues new componente lastUpdate using excel
</commit_message>
<xml_diff>
--- a/public/assets/users.xlsx
+++ b/public/assets/users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme\Desktop\JnJ-LATAM-Analytics\jnj\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89CC6258-BC68-408E-9D13-A96D74F7A537}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A807721-8CCE-4858-91E8-D51FF80925BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C0296DF4-C6B5-4EB4-BBB3-F97AF1587E4D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C0296DF4-C6B5-4EB4-BBB3-F97AF1587E4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -502,8 +502,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66D478EB-B1A3-4C29-98C1-830AEE2CAF1F}">
   <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
implements all users access
</commit_message>
<xml_diff>
--- a/public/assets/users.xlsx
+++ b/public/assets/users.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme\Desktop\JnJ-LATAM-Analytics\jnj\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A807721-8CCE-4858-91E8-D51FF80925BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22599E27-60A3-480E-85F4-06E072476EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{C0296DF4-C6B5-4EB4-BBB3-F97AF1587E4D}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C0296DF4-C6B5-4EB4-BBB3-F97AF1587E4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="84">
   <si>
     <t>Name</t>
   </si>
@@ -44,54 +44,15 @@
     <t>MedTech</t>
   </si>
   <si>
-    <t>suzy.jnj</t>
-  </si>
-  <si>
-    <t>ricardo.jnj</t>
-  </si>
-  <si>
-    <t>Sales</t>
-  </si>
-  <si>
-    <t>nikolas.jnj</t>
-  </si>
-  <si>
-    <t>renato.jnj</t>
-  </si>
-  <si>
     <t>Innovative Medicine</t>
   </si>
   <si>
-    <t>MedTech,Innovative Medicine,Vision Care,Surgical Vision</t>
-  </si>
-  <si>
     <t>Sales,Non sales</t>
   </si>
   <si>
-    <t>renato.gominho</t>
-  </si>
-  <si>
-    <t>ricardo.ohara</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
-    <t>suzy123</t>
-  </si>
-  <si>
-    <t>ricardo123</t>
-  </si>
-  <si>
-    <t>renato123</t>
-  </si>
-  <si>
-    <t>Suzy</t>
-  </si>
-  <si>
-    <t>Ricardo</t>
-  </si>
-  <si>
     <t>Renato</t>
   </si>
   <si>
@@ -110,9 +71,6 @@
     <t>Country</t>
   </si>
   <si>
-    <t>Brazil,Costa Rica,Republica Dominicana,Panama,Guatemala</t>
-  </si>
-  <si>
     <t>Brazil</t>
   </si>
   <si>
@@ -125,17 +83,218 @@
     <t>Sales,Non sales,Company Car,Authorized Driver, Authorized Driver - Events,Grey Fleet,Board</t>
   </si>
   <si>
-    <t>United States of America,Canada,Brazil,Argentina,Mexico,Puerto Rico,Puerto Rico NA,Colombia,Peru</t>
-  </si>
-  <si>
     <t>MedTech,Innovative Medicine,Vision Care,Surgical Vision,Global Services</t>
+  </si>
+  <si>
+    <t>smccray@its.jnj.com</t>
+  </si>
+  <si>
+    <t>Suzi</t>
+  </si>
+  <si>
+    <t>United States of America,Canada,Brazil,Argentina,Mexico,Puerto Rico,Puerto Rico NA,Colombia,Peru,Guatemala,Costa Rica,Dominican Republic,Chile,Panama,Ecuador,Uruguay,Venezuela</t>
+  </si>
+  <si>
+    <t>fmarque1its.jnj.com</t>
+  </si>
+  <si>
+    <t>Brazil,Argentina,Mexico,Puerto Rico,Puerto Rico NA,Colombia,Peru,Guatemala,Costa Rica,Dominican Republic,Chile,Panama,Ecuador,Uruguay,Venezuela</t>
+  </si>
+  <si>
+    <t>Flavio</t>
+  </si>
+  <si>
+    <t>Marcos</t>
+  </si>
+  <si>
+    <t>mgrandi@its.jnj.com</t>
+  </si>
+  <si>
+    <t>Argentina</t>
+  </si>
+  <si>
+    <t>Vision Care</t>
+  </si>
+  <si>
+    <t>acanosa@its.jnj.com</t>
+  </si>
+  <si>
+    <t>scalello@its.jnj.com</t>
+  </si>
+  <si>
+    <t>emarco1@its.jnj.com</t>
+  </si>
+  <si>
+    <t>André</t>
+  </si>
+  <si>
+    <t>Silvia</t>
+  </si>
+  <si>
+    <t>Eduardo</t>
+  </si>
+  <si>
+    <t>Surgical Vision</t>
+  </si>
+  <si>
+    <t>llemos2@its.jnj.com</t>
+  </si>
+  <si>
+    <t>rferna16@its.jnj.com</t>
+  </si>
+  <si>
+    <t>npadula@its.jnj.com</t>
+  </si>
+  <si>
+    <t>ddalalib@its.jnj.com</t>
+  </si>
+  <si>
+    <t>Luis</t>
+  </si>
+  <si>
+    <t>Nikolas</t>
+  </si>
+  <si>
+    <t>Daniel</t>
+  </si>
+  <si>
+    <t>Costa Rica</t>
+  </si>
+  <si>
+    <t>Dominican Republic</t>
+  </si>
+  <si>
+    <t>Guatemala</t>
+  </si>
+  <si>
+    <t>Panama</t>
+  </si>
+  <si>
+    <t>vreyes02@its.jnj.com</t>
+  </si>
+  <si>
+    <t>aalcan11@its.jnj.com</t>
+  </si>
+  <si>
+    <t>lperdom2@its.jnj.com</t>
+  </si>
+  <si>
+    <t>lvalle@its.jnj.com</t>
+  </si>
+  <si>
+    <t>malfaroa@its.jnj.com</t>
+  </si>
+  <si>
+    <t>mrivasga@its.jnj.com</t>
+  </si>
+  <si>
+    <t>Maria</t>
+  </si>
+  <si>
+    <t>Mayra</t>
+  </si>
+  <si>
+    <t>Vielka</t>
+  </si>
+  <si>
+    <t>Alfredo</t>
+  </si>
+  <si>
+    <t>Larissa</t>
+  </si>
+  <si>
+    <t>Chile</t>
+  </si>
+  <si>
+    <t>jgellona@its.jnj.com</t>
+  </si>
+  <si>
+    <t>magudelo@its.jnj.com</t>
+  </si>
+  <si>
+    <t>Andrés</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>Colombia</t>
+  </si>
+  <si>
+    <t>pnavaspi@its.jnj.com</t>
+  </si>
+  <si>
+    <t>erobles8@its.jnj.com</t>
+  </si>
+  <si>
+    <t>Mauricio</t>
+  </si>
+  <si>
+    <t>Eika</t>
+  </si>
+  <si>
+    <t>Paula</t>
+  </si>
+  <si>
+    <t>Ecuador</t>
+  </si>
+  <si>
+    <t>jpinoarg@its.jnj.com</t>
+  </si>
+  <si>
+    <t>José</t>
+  </si>
+  <si>
+    <t>Mexico</t>
+  </si>
+  <si>
+    <t>amoren15@its.jnj.com</t>
+  </si>
+  <si>
+    <t>jlcarida@its.jnj.com</t>
+  </si>
+  <si>
+    <t>galvirez@its.jnj.com</t>
+  </si>
+  <si>
+    <t>Jorge</t>
+  </si>
+  <si>
+    <t>Gabriel</t>
+  </si>
+  <si>
+    <t>Peru</t>
+  </si>
+  <si>
+    <t>Silvina</t>
+  </si>
+  <si>
+    <t>sromerog@its.jnj.com</t>
+  </si>
+  <si>
+    <t>Uruguay</t>
+  </si>
+  <si>
+    <t>Venezuela</t>
+  </si>
+  <si>
+    <t>Rafel</t>
+  </si>
+  <si>
+    <t>Jose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rsciarra@its.jnj.com </t>
+  </si>
+  <si>
+    <t>jgiron4@its.jnj.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,13 +302,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="9"/>
+      <color theme="4"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -161,13 +341,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -500,18 +688,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66D478EB-B1A3-4C29-98C1-830AEE2CAF1F}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.44140625" customWidth="1"/>
     <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="59.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="100.44140625" customWidth="1"/>
     <col min="5" max="5" width="76.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -521,146 +709,739 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>310300</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3">
+        <v>235689</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B4">
+        <v>124578</v>
+      </c>
+      <c r="C4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B5">
+        <v>142536</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B6">
+        <v>475869</v>
+      </c>
+      <c r="C6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
         <v>30</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" t="s">
-        <v>9</v>
-      </c>
-      <c r="F6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
+      <c r="B7">
+        <v>172839</v>
       </c>
       <c r="C7" t="s">
         <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="G7" t="s">
-        <v>21</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8">
+        <v>794613</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9">
+        <v>316497</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10">
+        <v>253698</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11">
+        <v>795843</v>
+      </c>
+      <c r="C11" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12">
+        <v>658793</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>50</v>
+      </c>
+      <c r="G12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13">
+        <v>968745</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14">
+        <v>998860</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15">
+        <v>458733</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G15" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16">
+        <v>987456</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" t="s">
+        <v>3</v>
+      </c>
+      <c r="F16" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17">
+        <v>123789</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18">
+        <v>987321</v>
+      </c>
+      <c r="C18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19">
+        <v>549813</v>
+      </c>
+      <c r="C19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" t="s">
+        <v>3</v>
+      </c>
+      <c r="F19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20">
+        <v>325678</v>
+      </c>
+      <c r="C20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" t="s">
+        <v>59</v>
+      </c>
+      <c r="G20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21">
+        <v>796513</v>
+      </c>
+      <c r="C21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" t="s">
+        <v>25</v>
+      </c>
+      <c r="E21" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22">
+        <v>464579</v>
+      </c>
+      <c r="C22" t="s">
+        <v>60</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>3</v>
+      </c>
+      <c r="F22" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23">
+        <v>645823</v>
+      </c>
+      <c r="C23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>3</v>
+      </c>
+      <c r="F23" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24">
+        <v>998536</v>
+      </c>
+      <c r="C24" t="s">
+        <v>66</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" t="s">
+        <v>68</v>
+      </c>
+      <c r="G24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25">
+        <v>885632</v>
+      </c>
+      <c r="C25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" t="s">
+        <v>25</v>
+      </c>
+      <c r="E25" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" t="s">
+        <v>53</v>
+      </c>
+      <c r="G25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26">
+        <v>974451</v>
+      </c>
+      <c r="C26" t="s">
+        <v>69</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>3</v>
+      </c>
+      <c r="F26" t="s">
+        <v>73</v>
+      </c>
+      <c r="G26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27">
+        <v>336985</v>
+      </c>
+      <c r="C27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27" t="s">
+        <v>74</v>
+      </c>
+      <c r="G27" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B28">
+        <v>885214</v>
+      </c>
+      <c r="C28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>3</v>
+      </c>
+      <c r="F28" t="s">
+        <v>76</v>
+      </c>
+      <c r="G28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>885273</v>
+      </c>
+      <c r="C29" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" t="s">
+        <v>3</v>
+      </c>
+      <c r="F29" t="s">
+        <v>30</v>
+      </c>
+      <c r="G29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30">
+        <v>997463</v>
+      </c>
+      <c r="C30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>3</v>
+      </c>
+      <c r="F30" t="s">
+        <v>80</v>
+      </c>
+      <c r="G30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B31">
+        <v>112873</v>
+      </c>
+      <c r="C31" t="s">
+        <v>79</v>
+      </c>
+      <c r="D31" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" t="s">
+        <v>3</v>
+      </c>
+      <c r="F31" t="s">
+        <v>81</v>
+      </c>
+      <c r="G31" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{3FEA065D-CBE5-434F-BBB7-950315966668}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{C0E47932-30C8-4032-9D0C-B906BEAEB248}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{618604E8-1449-47BB-8952-B36F22FCE988}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{2888DB44-7CA3-476E-89F9-40958724DB98}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{1F3CF379-7CD2-4596-9126-2377EE7DC53F}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{AF602163-337D-41A4-97C3-731C1D9637FD}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{74524030-17F6-4AA6-95E2-4E8A2545673B}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{DCFCDD9D-8244-4164-83AE-E26FE723A27E}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{1D7B83EB-892D-4A44-A83F-D8EEDCE05AB3}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{629FD280-0DCF-4DF1-8367-7CCA3B8224A6}"/>
+    <hyperlink ref="A12" r:id="rId11" xr:uid="{8C54B157-B9C7-434C-B0FF-BF22820C57DA}"/>
+    <hyperlink ref="A13" r:id="rId12" xr:uid="{9C32CBED-D87F-43A5-AE27-2ACC72DDE472}"/>
+    <hyperlink ref="A14" r:id="rId13" xr:uid="{EC0B7C13-A2AE-4982-876B-01D9CC62877A}"/>
+    <hyperlink ref="A15" r:id="rId14" xr:uid="{FFAF7014-9EB8-4DF1-A502-0DE007D2CD43}"/>
+    <hyperlink ref="A16" r:id="rId15" xr:uid="{046BF20A-07AD-4771-924D-7C13CD31097C}"/>
+    <hyperlink ref="A17" r:id="rId16" xr:uid="{9909989F-5607-4F18-A1DC-A7B9DC112B85}"/>
+    <hyperlink ref="A18" r:id="rId17" xr:uid="{89665F10-7509-4EAC-AFBB-52DC47D89CF0}"/>
+    <hyperlink ref="A20" r:id="rId18" xr:uid="{F9051B35-6861-4F2C-8978-CF632A23D577}"/>
+    <hyperlink ref="A21" r:id="rId19" xr:uid="{1A96B273-D733-42B1-A41D-62F17233AB9C}"/>
+    <hyperlink ref="A22" r:id="rId20" xr:uid="{F00005F8-2A00-4434-BCAE-C9D15A21EB2A}"/>
+    <hyperlink ref="A27" r:id="rId21" xr:uid="{1F54D127-0FCB-4556-BFC3-A04BE6D44778}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>